<commit_message>
uloha_02: Vytvoření modulu pro pomocné funkce
</commit_message>
<xml_diff>
--- a/uloha_02/data_02/data_02.xlsx
+++ b/uloha_02/data_02/data_02.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="teplota_absorpce" sheetId="1" state="visible" r:id="rId3"/>
@@ -59,11 +59,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -79,6 +80,17 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -123,12 +135,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -252,11 +268,16 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -470,17 +491,17 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="72211622"/>
-        <c:axId val="22893434"/>
+        <c:axId val="36574860"/>
+        <c:axId val="14766654"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72211622"/>
+        <c:axId val="36574860"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -497,17 +518,21 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22893434"/>
+        <c:crossAx val="14766654"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="22893434"/>
+        <c:axId val="14766654"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -522,7 +547,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -539,14 +564,18 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72211622"/>
+        <c:crossAx val="36574860"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -572,7 +601,11 @@
         <a:p>
           <a:pPr>
             <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:latin typeface="Arial"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:defRPr>
           </a:pPr>
         </a:p>
@@ -612,6 +645,587 @@
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>T [˚C]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>teplota_proud!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>675</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>635</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>495</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>299</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>teplota_proud!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>13.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="14559139"/>
+        <c:axId val="89732479"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="14559139"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="89732479"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="89732479"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="14559139"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:ea typeface="DejaVu Sans"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>teplota_proud!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>U_las [mV]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>teplota_proud!$C$2:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>249.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>229.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>199.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>174.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>137.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>109.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>79.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>54.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>34.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>teplota_proud!$D$2:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="96315068"/>
+        <c:axId val="20683314"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="96315068"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="20683314"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="20683314"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="96315068"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:ea typeface="DejaVu Sans"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>doba_zivota!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>U [mV]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -658,91 +1272,105 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>teplota_proud!$A$2:$A$11</c:f>
+              <c:f>doba_zivota!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>720</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>675</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>635</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>600</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>540</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>495</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>450</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>400</c:v>
+                  <c:v>280</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>350</c:v>
+                  <c:v>360</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>299</c:v>
+                  <c:v>552</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>teplota_proud!$B$2:$B$11</c:f>
+              <c:f>doba_zivota!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>13.1</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.1</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.6</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.4</c:v>
+                  <c:v>29.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.7</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.7</c:v>
+                  <c:v>22.4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18.6</c:v>
+                  <c:v>20.4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19.8</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20.9</c:v>
+                  <c:v>14.4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>21.7</c:v>
+                  <c:v>9.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="90895360"/>
-        <c:axId val="11091350"/>
+        <c:axId val="23357631"/>
+        <c:axId val="64665911"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="90895360"/>
+        <c:axId val="23357631"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -770,12 +1398,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11091350"/>
+        <c:crossAx val="64665911"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="11091350"/>
+        <c:axId val="64665911"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -812,272 +1440,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90895360"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="span"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="0">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>teplota_proud!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>U_las [mV]</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>teplota_proud!$C$2:$C$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>249.4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>229.4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>199.4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>174.4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>137.4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>109.4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>79.4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>54.4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>34.4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>16.4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>teplota_proud!$D$2:$D$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>148</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>116</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>103</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>76</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:axId val="99089490"/>
-        <c:axId val="20931737"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="99089490"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="20931737"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="20931737"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="0">
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="99089490"/>
+        <c:crossAx val="23357631"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1136,9 +1499,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>19080</xdr:colOff>
+      <xdr:colOff>18720</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>148680</xdr:rowOff>
+      <xdr:rowOff>148320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1147,7 +1510,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2542320" y="544320"/>
-        <a:ext cx="6417720" cy="3993480"/>
+        <a:ext cx="6417360" cy="3993120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1171,9 +1534,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>380880</xdr:colOff>
+      <xdr:colOff>380520</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>67320</xdr:rowOff>
+      <xdr:rowOff>66960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1182,7 +1545,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="5757840" y="78840"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:ext cx="5759280" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1201,9 +1564,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>404280</xdr:colOff>
+      <xdr:colOff>403920</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>99360</xdr:rowOff>
+      <xdr:rowOff>99000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1212,11 +1575,46 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="5780160" y="3689280"/>
-        <a:ext cx="5760720" cy="3237480"/>
+        <a:ext cx="5760360" cy="3237120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>43200</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>135360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>113040</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>123840</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="2481480" y="785520"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1339,259 +1737,259 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>6.1</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>452</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>7.5</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>373</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>202</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>11.5</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>129</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>11.9</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>119</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>118</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>12.1</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>118</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>12.2</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>119</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>12.5</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>123</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>145</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>235</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>15.3</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>470</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>16.6</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>800</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="1" t="n">
         <v>19.3</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>1365</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="1" t="n">
         <v>22.1</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>1400</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="1" t="n">
         <v>25.7</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>862</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+      <c r="A18" s="1" t="n">
         <v>27.8</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <v>605</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="A19" s="1" t="n">
         <v>28.2</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="1" t="n">
         <v>570</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+      <c r="A20" s="1" t="n">
         <v>28.7</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="1" t="n">
         <v>555</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="1" t="n">
         <v>555</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
+      <c r="A22" s="1" t="n">
         <v>29.6</v>
       </c>
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="1" t="n">
         <v>588</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
+      <c r="A23" s="1" t="n">
         <v>29.9</v>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="1" t="n">
         <v>603</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
+      <c r="A24" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B24" s="0" t="n">
+      <c r="B24" s="1" t="n">
         <v>613</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
+      <c r="A25" s="1" t="n">
         <v>31.8</v>
       </c>
-      <c r="B25" s="0" t="n">
+      <c r="B25" s="1" t="n">
         <v>915</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
+      <c r="A26" s="1" t="n">
         <v>35.2</v>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B26" s="1" t="n">
         <v>1775</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+      <c r="A27" s="1" t="n">
         <v>37.8</v>
       </c>
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="1" t="n">
         <v>2015</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
+      <c r="A28" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B28" s="0" t="n">
+      <c r="B28" s="1" t="n">
         <v>1862</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
+      <c r="A29" s="1" t="n">
         <v>42.5</v>
       </c>
-      <c r="B29" s="0" t="n">
+      <c r="B29" s="1" t="n">
         <v>1377</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
+      <c r="A30" s="1" t="n">
         <v>44.4</v>
       </c>
-      <c r="B30" s="0" t="n">
+      <c r="B30" s="1" t="n">
         <v>944</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
+      <c r="A31" s="1" t="n">
         <v>44.9</v>
       </c>
-      <c r="B31" s="0" t="n">
+      <c r="B31" s="1" t="n">
         <v>875</v>
       </c>
     </row>
@@ -1614,239 +2012,239 @@
   </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.62"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>720</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>13.1</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <f aca="false">F2-7.6</f>
         <v>249.4</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <f aca="false">E2-8</f>
         <v>148</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="2" t="n">
         <v>156</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>257</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>675</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>14.1</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <f aca="false">F3-7.6</f>
         <v>229.4</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <f aca="false">E3-8</f>
         <v>130</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="2" t="n">
         <v>138</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>237</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>635</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>14.6</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <f aca="false">F4-7.6</f>
         <v>199.4</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <f aca="false">E4-8</f>
         <v>116</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="2" t="n">
         <v>124</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <v>207</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>600</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>15.4</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <f aca="false">F5-7.6</f>
         <v>174.4</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <f aca="false">E5-8</f>
         <v>103</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="2" t="n">
         <v>111</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <v>182</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>540</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>16.7</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <f aca="false">F6-7.6</f>
         <v>137.4</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <f aca="false">E6-8</f>
         <v>76</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="2" t="n">
         <v>84</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <v>145</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>495</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>17.7</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <f aca="false">F7-7.6</f>
         <v>109.4</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <f aca="false">E7-8</f>
         <v>61</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="2" t="n">
         <v>69</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <v>117</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>450</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>18.6</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <f aca="false">F8-7.6</f>
         <v>79.4</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <f aca="false">E8-8</f>
         <v>42</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="1" t="n">
         <v>87</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>19.8</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <f aca="false">F9-7.6</f>
         <v>54.4</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <f aca="false">E9-8</f>
         <v>23</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" s="2" t="n">
         <v>31</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="1" t="n">
         <v>62</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>350</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>20.9</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <f aca="false">F10-7.6</f>
         <v>34.4</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <f aca="false">E10-8</f>
         <v>5</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="1" t="n">
         <v>42</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>299</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>21.7</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <f aca="false">F11-7.6</f>
         <v>16.4</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="1" t="n">
         <v>24</v>
       </c>
     </row>
@@ -1869,100 +2267,100 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>33</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>29.2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>160</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>22.4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>240</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>20.4</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>280</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>360</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>14.4</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>552</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>9.6</v>
       </c>
     </row>
@@ -1974,5 +2372,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Běžné"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Běžné"&amp;12Stránka &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>